<commit_message>
improved fuzzy: company name spelling mistake corrected
</commit_message>
<xml_diff>
--- a/compile/data/dhl_dummy_database_sz.xlsx
+++ b/compile/data/dhl_dummy_database_sz.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Documents\newcompile\compile\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70419E98-936E-4A1D-88EE-EC17A58F42A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40711B4E-E5F7-4C4F-ABA2-914AAC1C4D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8395" yWindow="19454" windowWidth="26301" windowHeight="14304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dhl_dummy_database_sz" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="190">
   <si>
     <t xml:space="preserve">Unique Lead Assignment Number </t>
   </si>
@@ -28,9 +38,6 @@
     <t>Lead Source Name</t>
   </si>
   <si>
-    <t>Lead Source Details, if any</t>
-  </si>
-  <si>
     <t>Suspect Creation date by Lead Originator</t>
   </si>
   <si>
@@ -58,9 +65,6 @@
     <t>Main Phone #</t>
   </si>
   <si>
-    <t>Contact Person Name</t>
-  </si>
-  <si>
     <t>Contact Person Email</t>
   </si>
   <si>
@@ -76,9 +80,6 @@
     <t>Physical Channel</t>
   </si>
   <si>
-    <t>SSM Number /Business Registration Number</t>
-  </si>
-  <si>
     <t>Competitors</t>
   </si>
   <si>
@@ -400,9 +401,6 @@
     <t>www.geometrydnb.com</t>
   </si>
   <si>
-    <t>B2B, B2C</t>
-  </si>
-  <si>
     <t>Interior Design</t>
   </si>
   <si>
@@ -535,9 +533,6 @@
     <t>info@iqiglobal.com</t>
   </si>
   <si>
-    <t>CEO</t>
-  </si>
-  <si>
     <t>www.iqiglobal.com</t>
   </si>
   <si>
@@ -566,13 +561,52 @@
   </si>
   <si>
     <t>Jin Huo Gold &amp; Jewellery Industries (M) Sdn. Bhd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSM Number /Business Registration Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Person Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Source Details , if any </t>
+  </si>
+  <si>
+    <t>IQI Holdingss Sdn Bhd</t>
+  </si>
+  <si>
+    <t>03-23323355</t>
+  </si>
+  <si>
+    <t>info@iqiglobasl.com</t>
+  </si>
+  <si>
+    <t>Ahmad Ali</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>cEo</t>
+  </si>
+  <si>
+    <t>03-11111111</t>
+  </si>
+  <si>
+    <t>Andrew Tate</t>
+  </si>
+  <si>
+    <t>andrewtate@iqiglobal.com</t>
+  </si>
+  <si>
+    <t>Social Media</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,6 +741,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1005,7 +1047,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1048,12 +1090,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1087,6 +1131,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1407,10 +1452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1463,8 @@
     <col min="4" max="4" width="6.5" customWidth="1"/>
     <col min="5" max="5" width="8.25" customWidth="1"/>
     <col min="6" max="6" width="43.125" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1428,121 +1475,121 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
       </c>
       <c r="K2">
         <v>14000</v>
       </c>
       <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="V2" t="s">
         <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" t="s">
-        <v>38</v>
       </c>
       <c r="AA2">
         <v>17</v>
@@ -1550,38 +1597,38 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3">
         <v>13600</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AA3">
         <v>17</v>
@@ -1589,47 +1636,47 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1"/>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4">
         <v>14100</v>
       </c>
       <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
         <v>50</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>51</v>
       </c>
-      <c r="N4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>54</v>
-      </c>
       <c r="R4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U4">
         <v>4899</v>
       </c>
       <c r="V4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AA4">
         <v>34</v>
@@ -1637,44 +1684,44 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K5">
         <v>14100</v>
       </c>
       <c r="L5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
         <v>59</v>
       </c>
-      <c r="M5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" t="s">
-        <v>61</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>62</v>
-      </c>
       <c r="R5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AA5">
         <v>75</v>
@@ -1682,47 +1729,47 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K6">
         <v>10050</v>
       </c>
       <c r="L6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s">
         <v>66</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>67</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" t="s">
         <v>68</v>
-      </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>70</v>
-      </c>
-      <c r="R6" t="s">
-        <v>37</v>
-      </c>
-      <c r="V6" t="s">
-        <v>71</v>
       </c>
       <c r="AA6">
         <v>5</v>
@@ -1730,47 +1777,47 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K7">
         <v>14100</v>
       </c>
       <c r="L7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" t="s">
         <v>74</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>75</v>
       </c>
-      <c r="N7" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>78</v>
-      </c>
       <c r="R7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U7">
         <v>443222</v>
       </c>
       <c r="V7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AA7">
         <v>96</v>
@@ -1778,44 +1825,44 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K8">
         <v>13600</v>
       </c>
       <c r="L8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" t="s">
         <v>82</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q8" t="s">
         <v>83</v>
       </c>
-      <c r="N8" t="s">
+      <c r="R8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" t="s">
         <v>84</v>
-      </c>
-      <c r="O8" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>86</v>
-      </c>
-      <c r="R8" t="s">
-        <v>37</v>
-      </c>
-      <c r="V8" t="s">
-        <v>87</v>
       </c>
       <c r="AA8">
         <v>105</v>
@@ -1823,47 +1870,47 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" t="s">
         <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" t="s">
-        <v>91</v>
       </c>
       <c r="K9">
         <v>31650</v>
       </c>
       <c r="L9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" t="s">
         <v>92</v>
       </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
         <v>93</v>
       </c>
-      <c r="N9" t="s">
+      <c r="R9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" t="s">
         <v>94</v>
-      </c>
-      <c r="O9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>96</v>
-      </c>
-      <c r="R9" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9" t="s">
-        <v>97</v>
       </c>
       <c r="AA9">
         <v>12</v>
@@ -1871,47 +1918,47 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" t="s">
         <v>98</v>
-      </c>
-      <c r="G10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" t="s">
-        <v>101</v>
       </c>
       <c r="K10">
         <v>8000</v>
       </c>
       <c r="L10" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" t="s">
         <v>102</v>
       </c>
-      <c r="M10" t="s">
+      <c r="Q10" t="s">
         <v>103</v>
       </c>
-      <c r="N10" t="s">
+      <c r="R10" t="s">
         <v>104</v>
       </c>
-      <c r="O10" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="V10" t="s">
         <v>105</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>106</v>
-      </c>
-      <c r="R10" t="s">
-        <v>107</v>
-      </c>
-      <c r="V10" t="s">
-        <v>108</v>
       </c>
       <c r="AA10">
         <v>4</v>
@@ -1919,47 +1966,47 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K11">
         <v>13600</v>
       </c>
       <c r="L11" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" t="s">
+        <v>111</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" t="s">
         <v>112</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>113</v>
       </c>
-      <c r="N11" t="s">
+      <c r="R11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" t="s">
         <v>114</v>
-      </c>
-      <c r="O11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>116</v>
-      </c>
-      <c r="R11" t="s">
-        <v>37</v>
-      </c>
-      <c r="V11" t="s">
-        <v>117</v>
       </c>
       <c r="AA11">
         <v>12</v>
@@ -1967,47 +2014,47 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K12">
         <v>10470</v>
       </c>
       <c r="L12" t="s">
+        <v>118</v>
+      </c>
+      <c r="M12" t="s">
+        <v>119</v>
+      </c>
+      <c r="O12" t="s">
+        <v>120</v>
+      </c>
+      <c r="P12" t="s">
         <v>121</v>
       </c>
-      <c r="M12" t="s">
+      <c r="Q12" t="s">
         <v>122</v>
       </c>
-      <c r="O12" t="s">
-        <v>123</v>
-      </c>
-      <c r="P12" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>125</v>
-      </c>
       <c r="R12" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="U12">
         <v>120</v>
       </c>
       <c r="V12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AA12">
         <v>27</v>
@@ -2015,38 +2062,38 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K13">
         <v>13600</v>
       </c>
       <c r="M13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="R13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AA13">
         <v>8</v>
@@ -2054,44 +2101,44 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I14" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K14">
         <v>13700</v>
       </c>
       <c r="L14" t="s">
+        <v>132</v>
+      </c>
+      <c r="M14" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" t="s">
+        <v>134</v>
+      </c>
+      <c r="O14" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q14" t="s">
         <v>136</v>
       </c>
-      <c r="M14" t="s">
+      <c r="R14" t="s">
+        <v>34</v>
+      </c>
+      <c r="V14" t="s">
         <v>137</v>
-      </c>
-      <c r="N14" t="s">
-        <v>138</v>
-      </c>
-      <c r="O14" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>140</v>
-      </c>
-      <c r="R14" t="s">
-        <v>37</v>
-      </c>
-      <c r="V14" t="s">
-        <v>141</v>
       </c>
       <c r="AA14">
         <v>800</v>
@@ -2099,44 +2146,44 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K15">
         <v>14100</v>
       </c>
       <c r="L15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="M15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="O15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="U15">
         <v>500</v>
       </c>
       <c r="V15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AA15">
         <v>26</v>
@@ -2144,86 +2191,86 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1"/>
       <c r="F16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K16">
         <v>11900</v>
       </c>
       <c r="L16" t="s">
+        <v>148</v>
+      </c>
+      <c r="M16" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" t="s">
+        <v>150</v>
+      </c>
+      <c r="O16" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>151</v>
+      </c>
+      <c r="R16" t="s">
+        <v>34</v>
+      </c>
+      <c r="V16" t="s">
         <v>152</v>
-      </c>
-      <c r="M16" t="s">
-        <v>153</v>
-      </c>
-      <c r="N16" t="s">
-        <v>154</v>
-      </c>
-      <c r="O16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>155</v>
-      </c>
-      <c r="R16" t="s">
-        <v>37</v>
-      </c>
-      <c r="V16" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K17">
         <v>14100</v>
       </c>
       <c r="L17" t="s">
+        <v>155</v>
+      </c>
+      <c r="M17" t="s">
+        <v>156</v>
+      </c>
+      <c r="N17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>158</v>
+      </c>
+      <c r="R17" t="s">
+        <v>34</v>
+      </c>
+      <c r="V17" t="s">
         <v>159</v>
-      </c>
-      <c r="M17" t="s">
-        <v>160</v>
-      </c>
-      <c r="N17" t="s">
-        <v>161</v>
-      </c>
-      <c r="O17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>162</v>
-      </c>
-      <c r="R17" t="s">
-        <v>37</v>
-      </c>
-      <c r="V17" t="s">
-        <v>163</v>
       </c>
       <c r="AA17">
         <v>17</v>
@@ -2231,89 +2278,89 @@
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G18" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I18" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="J18" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="K18">
-        <v>46200</v>
+        <v>13400</v>
       </c>
       <c r="L18" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="M18" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="N18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="O18" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="Q18" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R18" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="V18" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="AA18">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I19" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K19">
         <v>13400</v>
       </c>
       <c r="L19" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="M19" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="N19" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q19" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AA19">
         <v>80</v>
@@ -2321,44 +2368,44 @@
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G20" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K20">
         <v>13400</v>
       </c>
       <c r="L20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="M20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="N20" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q20" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AA20">
         <v>80</v>
@@ -2366,50 +2413,236 @@
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1"/>
       <c r="F21" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" t="s">
+        <v>161</v>
+      </c>
+      <c r="I21" t="s">
+        <v>162</v>
+      </c>
+      <c r="J21" t="s">
+        <v>163</v>
+      </c>
+      <c r="K21">
+        <v>46200</v>
+      </c>
+      <c r="L21" t="s">
         <v>181</v>
       </c>
-      <c r="G21" t="s">
-        <v>175</v>
-      </c>
-      <c r="I21" t="s">
-        <v>176</v>
-      </c>
-      <c r="J21" t="s">
-        <v>31</v>
-      </c>
-      <c r="K21">
-        <v>13400</v>
-      </c>
-      <c r="L21" t="s">
-        <v>177</v>
-      </c>
       <c r="M21" t="s">
-        <v>178</v>
-      </c>
-      <c r="N21" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="O21" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="Q21" t="s">
+        <v>167</v>
+      </c>
+      <c r="R21" t="s">
+        <v>104</v>
+      </c>
+      <c r="V21" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA21">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="F22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22">
+        <v>46200</v>
+      </c>
+      <c r="L22" t="s">
+        <v>181</v>
+      </c>
+      <c r="M22" t="s">
+        <v>183</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O22" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>167</v>
+      </c>
+      <c r="R22" t="s">
+        <v>104</v>
+      </c>
+      <c r="V22" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA22">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" t="s">
+        <v>163</v>
+      </c>
+      <c r="K23">
+        <v>46200</v>
+      </c>
+      <c r="L23" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>167</v>
+      </c>
+      <c r="R23" t="s">
+        <v>104</v>
+      </c>
+      <c r="V23" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" t="s">
+        <v>162</v>
+      </c>
+      <c r="J24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K24">
+        <v>46200</v>
+      </c>
+      <c r="L24" t="s">
+        <v>181</v>
+      </c>
+      <c r="M24" t="s">
+        <v>183</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O24" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>167</v>
+      </c>
+      <c r="R24" t="s">
+        <v>104</v>
+      </c>
+      <c r="V24" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA24">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="F25" t="s">
         <v>180</v>
       </c>
-      <c r="R21" t="s">
-        <v>37</v>
-      </c>
-      <c r="V21" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA21">
-        <v>80</v>
+      <c r="G25" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" t="s">
+        <v>162</v>
+      </c>
+      <c r="J25" t="s">
+        <v>163</v>
+      </c>
+      <c r="K25">
+        <v>46200</v>
+      </c>
+      <c r="L25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M25" t="s">
+        <v>187</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O25" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>167</v>
+      </c>
+      <c r="R25" t="s">
+        <v>104</v>
+      </c>
+      <c r="V25" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA25">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N21" r:id="rId1" xr:uid="{C7216A87-A59A-431C-8F8E-6B997CE8A7EF}"/>
+    <hyperlink ref="N24" r:id="rId2" xr:uid="{E007A358-394E-4735-8754-A3573DE2D2B7}"/>
+    <hyperlink ref="N22" r:id="rId3" xr:uid="{691A6E50-9F51-4698-AFA3-C1A7DEADDC17}"/>
+    <hyperlink ref="N25" r:id="rId4" xr:uid="{7825A658-CB2D-4FE0-8B4D-BDE77FF84559}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
read column name from csv in search.py
</commit_message>
<xml_diff>
--- a/compile/data/dhl_dummy_database_sz.xlsx
+++ b/compile/data/dhl_dummy_database_sz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Documents\newcompile\compile\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40711B4E-E5F7-4C4F-ABA2-914AAC1C4D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ECC38B-DFD1-48BA-B769-6C48A38E9549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="191">
   <si>
     <t xml:space="preserve">Unique Lead Assignment Number </t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>Social Media</t>
+  </si>
+  <si>
+    <t>geo@geomet.com</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1095,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1455,7 +1459,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2038,6 +2042,9 @@
       <c r="M12" t="s">
         <v>119</v>
       </c>
+      <c r="N12" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="O12" t="s">
         <v>120</v>
       </c>

</xml_diff>